<commit_message>
svar från tester, grafer,rapport
</commit_message>
<xml_diff>
--- a/dokument/statistik.xlsx
+++ b/dokument/statistik.xlsx
@@ -661,7 +661,7 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1117,106 +1117,106 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="D39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B40" s="1"/>
-      <c r="D40" s="2"/>
-      <c r="F40" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="D40" s="3">
+        <v>1282</v>
+      </c>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="D41" s="3">
-        <v>1282</v>
+        <v>35</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="D41" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1118</v>
+      </c>
       <c r="D42" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F42" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="1">
-        <v>1118</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="D43" s="3"/>
       <c r="F43" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B44" s="1"/>
-      <c r="D44" s="3"/>
-      <c r="F44" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="D44" s="3">
+        <v>1496</v>
+      </c>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B45" s="1"/>
-      <c r="D45" s="3">
-        <v>1496</v>
-      </c>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="1"/>
-      <c r="D46" s="1">
+      <c r="D45" s="1">
         <v>1300</v>
       </c>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>103</v>
       </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="D47" s="1">
+        <v>2014</v>
+      </c>
+      <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B48" s="1"/>
-      <c r="D48" s="1">
-        <v>2014</v>
-      </c>
-      <c r="F48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="F48" s="1">
+        <v>3175</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B49" s="1"/>
       <c r="D49" s="1"/>
@@ -1224,43 +1224,43 @@
         <v>3175</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>62</v>
+    <row r="50" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="B50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="F50" s="1">
-        <v>3175</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="1"/>
+      <c r="D50" s="3"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="D51" s="3"/>
-      <c r="F51" s="2"/>
+      <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="D52" s="3">
+        <v>1999</v>
+      </c>
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="1"/>
-      <c r="D53" s="3">
-        <v>1999</v>
-      </c>
-      <c r="F53" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">

</xml_diff>